<commit_message>
temporarily reverted parser due to bug
</commit_message>
<xml_diff>
--- a/sample_output.xlsx
+++ b/sample_output.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="38">
-  <si>
-    <t>YES picks</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="42">
+  <si>
+    <t>CMA picks</t>
   </si>
   <si>
     <t>20'</t>
@@ -37,7 +37,19 @@
     <t>Special</t>
   </si>
   <si>
-    <t>YES drops</t>
+    <t>CMA drops</t>
+  </si>
+  <si>
+    <t>APL picks</t>
+  </si>
+  <si>
+    <t>APL drops</t>
+  </si>
+  <si>
+    <t>ANL picks</t>
+  </si>
+  <si>
+    <t>ANL drops</t>
   </si>
   <si>
     <t>COS picks</t>
@@ -459,13 +471,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AU7"/>
+  <dimension ref="A1:BA7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:53">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,8 +574,20 @@
       <c r="AU1" t="s">
         <v>37</v>
       </c>
+      <c r="AW1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:53">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -579,6 +603,9 @@
       <c r="G2" t="s">
         <v>1</v>
       </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
       <c r="J2" t="s">
         <v>1</v>
       </c>
@@ -588,9 +615,6 @@
       <c r="M2" t="s">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
-        <v>1</v>
-      </c>
       <c r="P2" t="s">
         <v>1</v>
       </c>
@@ -612,32 +636,32 @@
       <c r="Y2" t="s">
         <v>1</v>
       </c>
+      <c r="Z2" t="s">
+        <v>1</v>
+      </c>
       <c r="AB2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AC2" t="s">
         <v>1</v>
       </c>
       <c r="AE2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI2" t="s">
         <v>1</v>
       </c>
       <c r="AK2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AN2" t="s">
         <v>1</v>
       </c>
-      <c r="AO2" t="s">
-        <v>1</v>
-      </c>
       <c r="AQ2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AR2" t="s">
         <v>1</v>
@@ -645,8 +669,20 @@
       <c r="AT2" t="s">
         <v>1</v>
       </c>
+      <c r="AU2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:53">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -662,6 +698,9 @@
       <c r="G3" t="s">
         <v>2</v>
       </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
       <c r="J3" t="s">
         <v>2</v>
       </c>
@@ -669,13 +708,10 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" t="s">
         <v>2</v>
       </c>
       <c r="P3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q3" t="s">
         <v>2</v>
@@ -693,37 +729,49 @@
         <v>2</v>
       </c>
       <c r="Y3" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>5</v>
       </c>
       <c r="AC3" t="s">
         <v>2</v>
       </c>
       <c r="AE3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI3" t="s">
         <v>2</v>
       </c>
       <c r="AK3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN3" t="s">
         <v>2</v>
       </c>
       <c r="AQ3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AR3" t="s">
         <v>2</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AU3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:53">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -739,10 +787,19 @@
       <c r="G4" t="s">
         <v>3</v>
       </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
       <c r="J4" t="s">
         <v>3</v>
       </c>
-      <c r="N4" t="s">
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
         <v>3</v>
       </c>
       <c r="Q4" t="s">
@@ -754,32 +811,38 @@
       <c r="W4" t="s">
         <v>3</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>3</v>
       </c>
       <c r="AC4" t="s">
         <v>3</v>
       </c>
-      <c r="AH4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AO4" t="s">
+      <c r="AE4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ4" t="s">
         <v>3</v>
       </c>
       <c r="AR4" t="s">
         <v>3</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AU4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:53">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -789,13 +852,22 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
       <c r="J5" t="s">
         <v>4</v>
       </c>
-      <c r="N5" t="s">
+      <c r="M5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
         <v>4</v>
       </c>
       <c r="Q5" t="s">
@@ -807,26 +879,32 @@
       <c r="W5" t="s">
         <v>4</v>
       </c>
-      <c r="Y5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AL5" t="s">
+      <c r="Z5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ5" t="s">
         <v>4</v>
       </c>
       <c r="AR5" t="s">
         <v>4</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AX5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:53">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -836,16 +914,22 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
       <c r="J6" t="s">
         <v>5</v>
       </c>
-      <c r="N6" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="M6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" t="s">
         <v>5</v>
       </c>
       <c r="T6" t="s">
@@ -854,45 +938,63 @@
       <c r="W6" t="s">
         <v>5</v>
       </c>
-      <c r="Y6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AT6" t="s">
+      <c r="Z6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AZ6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:53">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
-      <c r="J7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AT7" t="s">
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AZ7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>